<commit_message>
program correctly does the following: finds a random cell, finds a direction, finds a valid neighbor
</commit_message>
<xml_diff>
--- a/program4-logic.xlsx
+++ b/program4-logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlerch/Documents/school/fall23/it279/program4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB45B6A9-2EB1-0F42-B4BA-A18B6D006B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6213C84E-3F36-FA4F-B17C-6ABB99217CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
+    <workbookView xWindow="10100" yWindow="29540" windowWidth="30240" windowHeight="18900" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>for check if right is valid: false if rightIndex % numColumns == 0</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>calculate downIndex: origIndex + numColumns</t>
+  </si>
+  <si>
+    <t>make sure to set the cell wall variables correctly. For example orig west wall is really origLeft's east wall, unless orig is the left most cell in the row</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -101,12 +110,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A295FA-6DB9-1F41-B9A4-568A692DB912}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -440,7 +452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -451,12 +463,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -467,8 +479,12 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -477,8 +493,12 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,8 +509,12 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -501,8 +525,12 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -513,8 +541,12 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -523,8 +555,12 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -535,8 +571,12 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -547,8 +587,12 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -559,8 +603,12 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -571,8 +619,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -581,9 +633,15 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -591,6 +649,48 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Maze.h, Maze.cpp: program now removes walls and updates the disjoint set checking for the completed maze end condition
</commit_message>
<xml_diff>
--- a/program4-logic.xlsx
+++ b/program4-logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlerch/Documents/school/fall23/it279/program4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6213C84E-3F36-FA4F-B17C-6ABB99217CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708D6A7D-B16C-044C-B186-888D751C67D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10100" yWindow="29540" windowWidth="30240" windowHeight="18900" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A295FA-6DB9-1F41-B9A4-568A692DB912}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,6 +692,91 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>10</v>
+      </c>
+      <c r="B26" s="1">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1">
+        <v>16</v>
+      </c>
+      <c r="C27" s="1">
+        <v>17</v>
+      </c>
+      <c r="D27" s="1">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1">
+        <v>23</v>
+      </c>
+      <c r="E28" s="1">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
works for all provided sample mazes
</commit_message>
<xml_diff>
--- a/program4-logic.xlsx
+++ b/program4-logic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlerch/Documents/school/fall23/it279/program4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708D6A7D-B16C-044C-B186-888D751C67D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7972C75A-63D0-7044-96D9-27E5AD8639A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
+    <workbookView xWindow="10100" yWindow="29540" windowWidth="30240" windowHeight="18900" xr2:uid="{FBEC1579-E01E-7E45-9237-D919D8AF505E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>for check if right is valid: false if rightIndex % numColumns == 0</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>make sure to set the cell wall variables correctly. For example orig west wall is really origLeft's east wall, unless orig is the left most cell in the row</t>
+  </si>
+  <si>
+    <t>questions:</t>
+  </si>
+  <si>
+    <t>does not return cell in all cases warning. Could I just return currentCell at the end of the function or is that bad style</t>
+  </si>
+  <si>
+    <t>you mentioned that there could be an error that the sample files don't find. How do I check for that error?</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -106,17 +115,179 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,60 +604,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A295FA-6DB9-1F41-B9A4-568A692DB912}">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="B1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D2" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="3" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C3" s="9">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D3" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -497,11 +654,9 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -513,12 +668,12 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -529,12 +684,12 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -545,10 +700,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -559,11 +716,9 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -575,12 +730,12 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -591,12 +746,12 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -607,12 +762,12 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -623,10 +778,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -637,11 +794,9 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -653,127 +808,160 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="24" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" s="5">
         <v>0</v>
       </c>
-      <c r="B24" s="1">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D25" s="6">
         <v>2</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E25" s="6">
         <v>3</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F25" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B26" s="11">
         <v>5</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C26" s="4">
         <v>6</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D26" s="4">
         <v>7</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E26" s="4">
         <v>8</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F26" s="12">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B27" s="11">
         <v>10</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C27" s="4">
         <v>11</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D27" s="4">
         <v>12</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E27" s="4">
         <v>13</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F27" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B28" s="11">
         <v>15</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C28" s="4">
         <v>16</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D28" s="4">
         <v>17</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E28" s="4">
         <v>18</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F28" s="12">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+    <row r="29" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
         <v>20</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C29" s="9">
         <v>21</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D29" s="9">
         <v>22</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E29" s="9">
         <v>23</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F29" s="10">
         <v>24</v>
       </c>
     </row>

</xml_diff>